<commit_message>
Minimum treatment age 5
</commit_message>
<xml_diff>
--- a/sch_simulation/data/SCH_params/mansoni_coverage_scenario_1.xlsx
+++ b/sch_simulation/data/SCH_params/mansoni_coverage_scenario_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/sch/ntd-model-sch/sch_simulation/data/SCH_params/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC768E5A-F3FA-8049-8671-DCA634AD877F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E63891-620B-1649-89CB-4E9F1653E41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19200" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19180" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
   </bookViews>
   <sheets>
     <sheet name="Platform Coverage" sheetId="1" r:id="rId1"/>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC57624-070C-4C6C-8EF3-3B0C0B08BDC6}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -569,7 +569,7 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>14</v>
@@ -981,12 +981,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E3B750AFB9343D42B939C6ACF084A84C" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="93cd09b7eadf1f96f07e4cafc6f5cdf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00318829-ac19-4fa6-afcb-83e1ad4ea23b" xmlns:ns3="5ffa21b6-e00b-4719-91c3-427b29c2b057" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb8f100d907d4c7940a7c9646b5f1c73" ns2:_="" ns3:_="">
     <xsd:import namespace="00318829-ac19-4fa6-afcb-83e1ad4ea23b"/>
@@ -1203,6 +1197,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
   <ds:schemaRefs>
@@ -1212,15 +1212,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E6E6D53-A4AA-4BF4-8C61-16B862AC0A51}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1237,4 +1228,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correcting age bins for coverage
</commit_message>
<xml_diff>
--- a/sch_simulation/data/SCH_params/mansoni_coverage_scenario_1.xlsx
+++ b/sch_simulation/data/SCH_params/mansoni_coverage_scenario_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/sch/ntd-model-sch/sch_simulation/data/SCH_params/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E63891-620B-1649-89CB-4E9F1653E41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7B239E-9A97-A64A-A62A-E899AFC45A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19180" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
   </bookViews>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC57624-070C-4C6C-8EF3-3B0C0B08BDC6}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -572,7 +572,7 @@
         <v>5</v>
       </c>
       <c r="G2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2">
         <v>0.6</v>
@@ -628,7 +628,7 @@
         <v>15</v>
       </c>
       <c r="G3">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
@@ -688,7 +688,7 @@
         <v>5</v>
       </c>
       <c r="G6">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
@@ -972,6 +972,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -980,7 +986,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E3B750AFB9343D42B939C6ACF084A84C" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="93cd09b7eadf1f96f07e4cafc6f5cdf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00318829-ac19-4fa6-afcb-83e1ad4ea23b" xmlns:ns3="5ffa21b6-e00b-4719-91c3-427b29c2b057" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb8f100d907d4c7940a7c9646b5f1c73" ns2:_="" ns3:_="">
     <xsd:import namespace="00318829-ac19-4fa6-afcb-83e1ad4ea23b"/>
@@ -1197,13 +1203,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1211,7 +1220,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E6E6D53-A4AA-4BF4-8C61-16B862AC0A51}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1228,13 +1237,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated scenario 1 coverage
Minimum age is 5
No missing ages in coverage
</commit_message>
<xml_diff>
--- a/sch_simulation/data/SCH_params/mansoni_coverage_scenario_1.xlsx
+++ b/sch_simulation/data/SCH_params/mansoni_coverage_scenario_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/sch/ntd-model-sch/sch_simulation/data/SCH_params/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\ntd-model-sch\sch_simulation\data\SCH_params\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC768E5A-F3FA-8049-8671-DCA634AD877F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3663E3B7-81D1-4866-920C-216565412247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19200" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="18000" windowHeight="9150" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
   </bookViews>
   <sheets>
     <sheet name="Platform Coverage" sheetId="1" r:id="rId1"/>
@@ -450,20 +450,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC57624-070C-4C6C-8EF3-3B0C0B08BDC6}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="7" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,7 +555,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -569,10 +569,10 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2">
         <v>0.6</v>
@@ -611,7 +611,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -628,10 +628,10 @@
         <v>15</v>
       </c>
       <c r="G3">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -651,7 +651,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -671,7 +671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -691,7 +691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -724,12 +724,12 @@
       <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -809,7 +809,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -820,7 +820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -900,7 +900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -911,7 +911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -922,7 +922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -933,7 +933,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -944,7 +944,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -955,7 +955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -972,21 +972,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E3B750AFB9343D42B939C6ACF084A84C" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="93cd09b7eadf1f96f07e4cafc6f5cdf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00318829-ac19-4fa6-afcb-83e1ad4ea23b" xmlns:ns3="5ffa21b6-e00b-4719-91c3-427b29c2b057" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb8f100d907d4c7940a7c9646b5f1c73" ns2:_="" ns3:_="">
     <xsd:import namespace="00318829-ac19-4fa6-afcb-83e1ad4ea23b"/>
@@ -1203,24 +1188,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E6E6D53-A4AA-4BF4-8C61-16B862AC0A51}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1237,4 +1220,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to prop never treated and coverage times
</commit_message>
<xml_diff>
--- a/sch_simulation/data/SCH_params/mansoni_coverage_scenario_1.xlsx
+++ b/sch_simulation/data/SCH_params/mansoni_coverage_scenario_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\ntd-model-sch\sch_simulation\data\SCH_params\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3663E3B7-81D1-4866-920C-216565412247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FA9D49-A4E5-4825-B59F-E7FE884DC8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="18000" windowHeight="9150" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2B23B0C0-4BFB-41FB-ACE5-EE30D4858695}"/>
   </bookViews>
   <sheets>
     <sheet name="Platform Coverage" sheetId="1" r:id="rId1"/>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC57624-070C-4C6C-8EF3-3B0C0B08BDC6}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,34 +577,67 @@
       <c r="H2">
         <v>0.6</v>
       </c>
+      <c r="I2">
+        <v>0.6</v>
+      </c>
       <c r="J2">
         <v>0.6</v>
       </c>
+      <c r="K2">
+        <v>0.6</v>
+      </c>
       <c r="L2">
         <v>0.6</v>
       </c>
+      <c r="M2">
+        <v>0.6</v>
+      </c>
       <c r="N2">
         <v>0.6</v>
       </c>
+      <c r="O2">
+        <v>0.6</v>
+      </c>
       <c r="P2">
         <v>0.6</v>
       </c>
+      <c r="Q2">
+        <v>0.6</v>
+      </c>
       <c r="R2">
         <v>0.6</v>
       </c>
+      <c r="S2">
+        <v>0.6</v>
+      </c>
       <c r="T2">
         <v>0.6</v>
       </c>
+      <c r="U2">
+        <v>0.6</v>
+      </c>
       <c r="V2">
         <v>0.6</v>
       </c>
+      <c r="W2">
+        <v>0.6</v>
+      </c>
       <c r="X2">
         <v>0.6</v>
       </c>
+      <c r="Y2">
+        <v>0.6</v>
+      </c>
       <c r="Z2">
         <v>0.6</v>
       </c>
+      <c r="AA2">
+        <v>0.6</v>
+      </c>
       <c r="AB2">
+        <v>0.6</v>
+      </c>
+      <c r="AC2">
         <v>0.6</v>
       </c>
       <c r="AD2">
@@ -972,6 +1005,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E3B750AFB9343D42B939C6ACF084A84C" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="93cd09b7eadf1f96f07e4cafc6f5cdf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00318829-ac19-4fa6-afcb-83e1ad4ea23b" xmlns:ns3="5ffa21b6-e00b-4719-91c3-427b29c2b057" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb8f100d907d4c7940a7c9646b5f1c73" ns2:_="" ns3:_="">
     <xsd:import namespace="00318829-ac19-4fa6-afcb-83e1ad4ea23b"/>
@@ -1188,12 +1227,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1204,6 +1237,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E6E6D53-A4AA-4BF4-8C61-16B862AC0A51}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1222,15 +1264,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E0411F9-2A1E-4488-925A-5AD296329D24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6338434B-B586-489B-A269-E3728BE15AC4}">
   <ds:schemaRefs>

</xml_diff>